<commit_message>
This commit is for Part-4
</commit_message>
<xml_diff>
--- a/part-2 perform subnetting & basic router config/subnetting of all port.xlsx
+++ b/part-2 perform subnetting & basic router config/subnetting of all port.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\CiscoPacketTracer\part-2 perform subnetting &amp; basic router config\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F34A9C59-E469-4118-A910-16D36D4A5E8B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1EBCD0D-573D-4059-8626-9E78A8CA3BEF}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{C61DD1E7-C80E-488A-8AFA-0C50E3D193F3}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="73">
   <si>
     <t>IP's</t>
   </si>
@@ -228,16 +228,29 @@
 255.255.255.224</t>
   </si>
   <si>
-    <t>/31
-255.255.255.254</t>
-  </si>
-  <si>
     <t>/26
 255.255.255.192</t>
   </si>
   <si>
     <t>/25
 255.255.255.128</t>
+  </si>
+  <si>
+    <t>/30
+255.255.255.254</t>
+  </si>
+  <si>
+    <t>Unknown Network</t>
+  </si>
+  <si>
+    <t>Next Hop/Router IP Address</t>
+  </si>
+  <si>
+    <t>WAN-1 190.10.5.224/30</t>
+  </si>
+  <si>
+    <t>Se 0/1/1 190.10.5.244
+(R2)</t>
   </si>
 </sst>
 </file>
@@ -292,7 +305,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -330,13 +343,22 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -352,6 +374,15 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="2" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -669,283 +700,291 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AE7772A4-FDE4-4846-AE58-BC2563D9EA9E}">
-  <dimension ref="A1:I19"/>
+  <dimension ref="A1:K14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K14" sqref="K14"/>
+      <selection activeCell="J8" sqref="J8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="15.21875" customWidth="1"/>
-    <col min="5" max="5" width="15.88671875" customWidth="1"/>
-    <col min="6" max="6" width="15.5546875" customWidth="1"/>
-    <col min="7" max="7" width="14.21875" customWidth="1"/>
-    <col min="8" max="8" width="14.6640625" customWidth="1"/>
-    <col min="9" max="9" width="16.6640625" customWidth="1"/>
+    <col min="2" max="2" width="7.21875" customWidth="1"/>
+    <col min="3" max="3" width="6" customWidth="1"/>
+    <col min="4" max="4" width="16.109375" customWidth="1"/>
+    <col min="5" max="5" width="13.6640625" customWidth="1"/>
+    <col min="6" max="6" width="14.33203125" customWidth="1"/>
+    <col min="7" max="7" width="14" customWidth="1"/>
+    <col min="8" max="8" width="16.21875" customWidth="1"/>
+    <col min="9" max="9" width="5" customWidth="1"/>
+    <col min="10" max="10" width="28" style="8" customWidth="1"/>
+    <col min="11" max="11" width="25.77734375" style="8" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1"/>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2" s="6" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3" s="6" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A4" s="6" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="E8" s="1"/>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="E9" s="1"/>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="E10" s="1"/>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="B11" s="4" t="s">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A6" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="C11" s="4" t="s">
+      <c r="B6" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="D11" s="4" t="s">
+      <c r="C6" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="E11" s="4" t="s">
+      <c r="D6" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="F11" s="4" t="s">
+      <c r="E6" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="G11" s="4" t="s">
+      <c r="F6" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="H11" s="4" t="s">
+      <c r="G6" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="I11" s="4" t="s">
+      <c r="H6" s="4" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="12" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="B12" s="2" t="s">
+      <c r="J6" s="9" t="s">
+        <v>69</v>
+      </c>
+      <c r="K6" s="9" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" ht="31.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="2" t="s">
         <v>15</v>
       </c>
+      <c r="B7" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="D7" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="G7" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="H7" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="J7" s="8" t="s">
+        <v>71</v>
+      </c>
+      <c r="K7" s="10" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" ht="31.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="D8" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="G8" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="H8" s="2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="D9" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="F9" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="G9" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="H9" s="2" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" ht="29.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="D10" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="F10" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="G10" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="H10" s="2" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" ht="27.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="D11" s="7" t="s">
+        <v>65</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="F11" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="G11" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="H11" s="2" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B12" s="3">
+        <v>2</v>
+      </c>
       <c r="C12" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="D12" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="E12" s="7" t="s">
-        <v>63</v>
+        <v>50</v>
+      </c>
+      <c r="D12" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>51</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>21</v>
+        <v>52</v>
       </c>
       <c r="G12" s="2" t="s">
-        <v>22</v>
+        <v>53</v>
       </c>
       <c r="H12" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="I12" s="2" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="B13" s="2" t="s">
-        <v>16</v>
+        <v>54</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" ht="27.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B13" s="3">
+        <v>2</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="D13" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="E13" s="7" t="s">
-        <v>64</v>
+        <v>50</v>
+      </c>
+      <c r="D13" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>55</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>28</v>
+        <v>56</v>
       </c>
       <c r="G13" s="2" t="s">
-        <v>29</v>
+        <v>57</v>
       </c>
       <c r="H13" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="I13" s="2" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="B14" s="2" t="s">
-        <v>17</v>
+        <v>58</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" ht="31.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B14" s="3">
+        <v>2</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="D14" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="E14" s="7" t="s">
-        <v>67</v>
+        <v>50</v>
+      </c>
+      <c r="D14" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="E14" s="2" t="s">
+        <v>59</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>34</v>
+        <v>60</v>
       </c>
       <c r="G14" s="2" t="s">
-        <v>35</v>
+        <v>61</v>
       </c>
       <c r="H14" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="I14" s="2" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="B15" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="C15" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="D15" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="E15" s="7" t="s">
-        <v>68</v>
-      </c>
-      <c r="F15" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="G15" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="H15" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="I15" s="2" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="B16" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="C16" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="D16" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="E16" s="7" t="s">
-        <v>65</v>
-      </c>
-      <c r="F16" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="G16" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="H16" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="I16" s="2" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="17" spans="2:9" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="B17" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="C17" s="3">
-        <v>2</v>
-      </c>
-      <c r="D17" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="E17" s="7" t="s">
-        <v>66</v>
-      </c>
-      <c r="F17" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="G17" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="H17" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="I17" s="2" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="18" spans="2:9" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="B18" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C18" s="3">
-        <v>2</v>
-      </c>
-      <c r="D18" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="E18" s="7" t="s">
-        <v>66</v>
-      </c>
-      <c r="F18" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="G18" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="H18" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="I18" s="2" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="19" spans="2:9" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="B19" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="C19" s="3">
-        <v>2</v>
-      </c>
-      <c r="D19" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="E19" s="7" t="s">
-        <v>66</v>
-      </c>
-      <c r="F19" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="G19" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="H19" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="I19" s="2" t="s">
         <v>62</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Edited Subneting of WAN's
</commit_message>
<xml_diff>
--- a/part-2 perform subnetting & basic router config/subnetting of all port.xlsx
+++ b/part-2 perform subnetting & basic router config/subnetting of all port.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\CiscoPacketTracer\part-2 perform subnetting &amp; basic router config\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1EBCD0D-573D-4059-8626-9E78A8CA3BEF}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49A919D1-10C3-47CA-9B35-666BB8654660}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{C61DD1E7-C80E-488A-8AFA-0C50E3D193F3}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="69">
   <si>
     <t>IP's</t>
   </si>
@@ -237,20 +237,7 @@
   </si>
   <si>
     <t>/30
-255.255.255.254</t>
-  </si>
-  <si>
-    <t>Unknown Network</t>
-  </si>
-  <si>
-    <t>Next Hop/Router IP Address</t>
-  </si>
-  <si>
-    <t>WAN-1 190.10.5.224/30</t>
-  </si>
-  <si>
-    <t>Se 0/1/1 190.10.5.244
-(R2)</t>
+255.255.255.252</t>
   </si>
 </sst>
 </file>
@@ -358,7 +345,7 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -380,9 +367,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -703,7 +687,7 @@
   <dimension ref="A1:K14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J8" sqref="J8"/>
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -767,12 +751,8 @@
       <c r="H6" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="J6" s="9" t="s">
-        <v>69</v>
-      </c>
-      <c r="K6" s="9" t="s">
-        <v>70</v>
-      </c>
+      <c r="J6" s="9"/>
+      <c r="K6" s="9"/>
     </row>
     <row r="7" spans="1:11" ht="31.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
@@ -799,12 +779,7 @@
       <c r="H7" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="J7" s="8" t="s">
-        <v>71</v>
-      </c>
-      <c r="K7" s="10" t="s">
-        <v>72</v>
-      </c>
+      <c r="K7" s="9"/>
     </row>
     <row r="8" spans="1:11" ht="31.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">

</xml_diff>